<commit_message>
Update NA color and ignore temp Excel files
Changed the NA color in vis_scores.R from 'no_data' to 'not_applicable' for improved clarity. Updated .gitignore to exclude temporary Excel files. Updated the sample WHO Seasonal Risk Assessment Tool data file.
</commit_message>
<xml_diff>
--- a/data/WHO Seasonal Risk Assessment Tool (SAMPLE).xlsx
+++ b/data/WHO Seasonal Risk Assessment Tool (SAMPLE).xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11214"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve.kerr/Documents/GitHub/riskassess/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC83C97-AF1B-6949-AC92-ACFC8F8362F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CB575A-F822-D647-B4B7-B3220AB565D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10160" yWindow="-20200" windowWidth="30240" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17120" yWindow="-20980" windowWidth="38400" windowHeight="20980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Introduction" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="1" r:id="rId1"/>
     <sheet name="Indicator Metadata" sheetId="8" r:id="rId2"/>
     <sheet name="Indicator Data" sheetId="12" r:id="rId3"/>
     <sheet name="Pillar Weights" sheetId="15" r:id="rId4"/>
@@ -10446,7 +10446,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10530,8 +10530,15 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10550,6 +10557,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -10564,7 +10577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -10636,18 +10649,6 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -10663,6 +10664,19 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11231,6 +11245,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFD9EAD3"/>
+      <color rgb="FFFCE5CD"/>
+      <color rgb="FFCFE2F3"/>
+      <color rgb="FFE6E6E6"/>
       <color rgb="FF6CC24A"/>
       <color rgb="FFF5A623"/>
       <color rgb="FF00ACA4"/>
@@ -11664,10 +11682,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FFE6E6E6"/>
+  </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11683,11 +11704,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="238.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -11745,11 +11766,11 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11763,10 +11784,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BEE362-3726-294D-A7B5-2EE1005515FF}">
+  <sheetPr>
+    <tabColor rgb="FFCFE2F3"/>
+  </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="116" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="117" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12181,10 +12205,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAFDAEB-B23B-E342-945F-36389A57F9E9}">
+  <sheetPr>
+    <tabColor rgb="FFCFE2F3"/>
+  </sheetPr>
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="31.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12348,7 +12375,7 @@
         <v>LOCC</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="139" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="137" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>49</v>
       </c>
@@ -13197,18 +13224,10 @@
       <c r="B17" s="1" t="str">
         <v>Luhanska</v>
       </c>
-      <c r="C17" s="28">
-        <v>5</v>
-      </c>
-      <c r="D17" s="28">
-        <v>2</v>
-      </c>
-      <c r="E17" s="28">
-        <v>1</v>
-      </c>
-      <c r="F17" s="28">
-        <v>5</v>
-      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
@@ -13216,15 +13235,9 @@
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
-      <c r="N17" s="28">
-        <v>5</v>
-      </c>
-      <c r="O17" s="28">
-        <v>5</v>
-      </c>
-      <c r="P17" s="28">
-        <v>3</v>
-      </c>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
       <c r="Q17" s="28"/>
     </row>
     <row r="18" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -13961,10 +13974,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B24BD2-9501-C24C-9544-CE39A2D144F0}">
+  <sheetPr>
+    <tabColor rgb="FFFCE5CD"/>
+  </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="220" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14030,15 +14046,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2441B2A0-8B31-BB4F-89F5-DCCD4E7A3D81}">
+  <sheetPr>
+    <tabColor rgb="FFFCE5CD"/>
+  </sheetPr>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="19" bestFit="1" customWidth="1"/>
@@ -14060,7 +14079,7 @@
         <v>46</v>
       </c>
       <c r="B2" s="19">
-        <f>SUMIF(C:C, A2,E:E)</f>
+        <f>SUMIF(C:C, A2,E:E )</f>
         <v>1</v>
       </c>
     </row>
@@ -14102,7 +14121,7 @@
         <v>3391</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="str" cm="1">
         <f t="array" ref="A10:C24">_xlfn._xlws.FILTER(
     Indicator_Metadata[[Indicator]:[Pillar]],
@@ -14128,7 +14147,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="str">
         <v>Elderly population (60 and Above)</v>
       </c>
@@ -14194,7 +14213,7 @@
         <v>6.9999999999999993E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="str">
         <v>Internally displaced people (IDP)</v>
       </c>
@@ -14238,7 +14257,7 @@
         <v>6.9999999999999993E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="str">
         <v>Unable to access health services</v>
       </c>
@@ -14260,7 +14279,7 @@
         <v>2.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="str">
         <v>Unable to get necessary medicine</v>
       </c>
@@ -14451,10 +14470,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F83AB1-6550-4F41-801E-D3FCC94B7941}">
-  <dimension ref="A1:Q34"/>
+  <sheetPr>
+    <tabColor rgb="FFD9EAD3"/>
+  </sheetPr>
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="113" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView topLeftCell="A2" zoomScale="118" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14467,8 +14489,8 @@
     <col min="18" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="67" x14ac:dyDescent="0.2">
-      <c r="C1" s="39" t="str" cm="1">
+    <row r="1" spans="1:20" ht="67" x14ac:dyDescent="0.2">
+      <c r="C1" s="35" t="str" cm="1">
         <f t="array" ref="C1">TRANSPOSE(
     _xlfn.XLOOKUP(
         C3,
@@ -14478,7 +14500,7 @@
 )</f>
         <v>Exposure</v>
       </c>
-      <c r="D1" s="39" t="str" cm="1">
+      <c r="D1" s="35" t="str" cm="1">
         <f t="array" ref="D1">TRANSPOSE(
     _xlfn.XLOOKUP(
         C3,
@@ -14488,7 +14510,7 @@
 )</f>
         <v>Exposure</v>
       </c>
-      <c r="E1" s="39" t="str" cm="1">
+      <c r="E1" s="35" t="str" cm="1">
         <f t="array" ref="E1">TRANSPOSE(
     _xlfn.XLOOKUP(
         D3,
@@ -14498,7 +14520,7 @@
 )</f>
         <v>Vulnerability</v>
       </c>
-      <c r="F1" s="39" t="str" cm="1">
+      <c r="F1" s="35" t="str" cm="1">
         <f t="array" ref="F1">TRANSPOSE(
     _xlfn.XLOOKUP(
         E3,
@@ -14508,7 +14530,7 @@
 )</f>
         <v>Vulnerability</v>
       </c>
-      <c r="G1" s="39" t="str" cm="1">
+      <c r="G1" s="35" t="str" cm="1">
         <f t="array" ref="G1">TRANSPOSE(
     _xlfn.XLOOKUP(
         F3,
@@ -14518,7 +14540,7 @@
 )</f>
         <v>Vulnerability</v>
       </c>
-      <c r="H1" s="39" t="str" cm="1">
+      <c r="H1" s="35" t="str" cm="1">
         <f t="array" ref="H1">TRANSPOSE(
     _xlfn.XLOOKUP(
         G3,
@@ -14528,7 +14550,7 @@
 )</f>
         <v>Vulnerability</v>
       </c>
-      <c r="I1" s="39" t="str" cm="1">
+      <c r="I1" s="35" t="str" cm="1">
         <f t="array" ref="I1">TRANSPOSE(
     _xlfn.XLOOKUP(
         H3,
@@ -14538,7 +14560,7 @@
 )</f>
         <v>Vulnerability</v>
       </c>
-      <c r="J1" s="39" t="str" cm="1">
+      <c r="J1" s="35" t="str" cm="1">
         <f t="array" ref="J1">TRANSPOSE(
     _xlfn.XLOOKUP(
         I3,
@@ -14548,7 +14570,7 @@
 )</f>
         <v>LOCC</v>
       </c>
-      <c r="K1" s="39" t="str" cm="1">
+      <c r="K1" s="35" t="str" cm="1">
         <f t="array" ref="K1">TRANSPOSE(
     _xlfn.XLOOKUP(
         J3,
@@ -14558,7 +14580,7 @@
 )</f>
         <v>LOCC</v>
       </c>
-      <c r="L1" s="39" t="str" cm="1">
+      <c r="L1" s="35" t="str" cm="1">
         <f t="array" ref="L1">TRANSPOSE(
     _xlfn.XLOOKUP(
         K3,
@@ -14568,7 +14590,7 @@
 )</f>
         <v>LOCC</v>
       </c>
-      <c r="M1" s="39" t="str" cm="1">
+      <c r="M1" s="35" t="str" cm="1">
         <f t="array" ref="M1">TRANSPOSE(
     _xlfn.XLOOKUP(
         L3,
@@ -14578,7 +14600,7 @@
 )</f>
         <v>LOCC</v>
       </c>
-      <c r="N1" s="39" t="str" cm="1">
+      <c r="N1" s="35" t="str" cm="1">
         <f t="array" ref="N1">TRANSPOSE(
     _xlfn.XLOOKUP(
         M3,
@@ -14588,7 +14610,7 @@
 )</f>
         <v>LOCC</v>
       </c>
-      <c r="O1" s="39" t="str" cm="1">
+      <c r="O1" s="35" t="str" cm="1">
         <f t="array" ref="O1">TRANSPOSE(
     _xlfn.XLOOKUP(
         N3,
@@ -14598,7 +14620,7 @@
 )</f>
         <v>LOCC</v>
       </c>
-      <c r="P1" s="39" t="str" cm="1">
+      <c r="P1" s="35" t="str" cm="1">
         <f t="array" ref="P1">TRANSPOSE(
     _xlfn.XLOOKUP(
         O3,
@@ -14608,7 +14630,7 @@
 )</f>
         <v>LOCC</v>
       </c>
-      <c r="Q1" s="39" t="str" cm="1">
+      <c r="Q1" s="35" t="str" cm="1">
         <f t="array" ref="Q1">TRANSPOSE(
     _xlfn.XLOOKUP(
         P3,
@@ -14619,8 +14641,8 @@
         <v>LOCC</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="138" x14ac:dyDescent="0.2">
-      <c r="C2" s="39" t="str" cm="1">
+    <row r="2" spans="1:20" ht="137" x14ac:dyDescent="0.2">
+      <c r="C2" s="35" t="str" cm="1">
         <f t="array" ref="C2">TRANSPOSE(
     _xlfn.XLOOKUP(
         C3,
@@ -14630,7 +14652,7 @@
 )</f>
         <v>Hazard</v>
       </c>
-      <c r="D2" s="39" t="str" cm="1">
+      <c r="D2" s="35" t="str" cm="1">
         <f t="array" ref="D2">TRANSPOSE(
     _xlfn.XLOOKUP(
         D3,
@@ -14640,7 +14662,7 @@
 )</f>
         <v>Vulnerable Population</v>
       </c>
-      <c r="E2" s="39" t="str" cm="1">
+      <c r="E2" s="35" t="str" cm="1">
         <f t="array" ref="E2">TRANSPOSE(
     _xlfn.XLOOKUP(
         E3,
@@ -14650,7 +14672,7 @@
 )</f>
         <v>Vulnerable Population</v>
       </c>
-      <c r="F2" s="39" t="str" cm="1">
+      <c r="F2" s="35" t="str" cm="1">
         <f t="array" ref="F2">TRANSPOSE(
     _xlfn.XLOOKUP(
         F3,
@@ -14660,7 +14682,7 @@
 )</f>
         <v>Vulnerable Population</v>
       </c>
-      <c r="G2" s="39" t="str" cm="1">
+      <c r="G2" s="35" t="str" cm="1">
         <f t="array" ref="G2">TRANSPOSE(
     _xlfn.XLOOKUP(
         G3,
@@ -14670,7 +14692,7 @@
 )</f>
         <v>Socioeconomic</v>
       </c>
-      <c r="H2" s="39" t="str" cm="1">
+      <c r="H2" s="35" t="str" cm="1">
         <f t="array" ref="H2">TRANSPOSE(
     _xlfn.XLOOKUP(
         H3,
@@ -14680,7 +14702,7 @@
 )</f>
         <v>Socioeconomic</v>
       </c>
-      <c r="I2" s="39" t="str" cm="1">
+      <c r="I2" s="35" t="str" cm="1">
         <f t="array" ref="I2">TRANSPOSE(
     _xlfn.XLOOKUP(
         I3,
@@ -14690,7 +14712,7 @@
 )</f>
         <v>Health Service Accessibility</v>
       </c>
-      <c r="J2" s="39" t="str" cm="1">
+      <c r="J2" s="35" t="str" cm="1">
         <f t="array" ref="J2">TRANSPOSE(
     _xlfn.XLOOKUP(
         J3,
@@ -14700,7 +14722,7 @@
 )</f>
         <v>Health Service Accessibility</v>
       </c>
-      <c r="K2" s="39" t="str" cm="1">
+      <c r="K2" s="35" t="str" cm="1">
         <f t="array" ref="K2">TRANSPOSE(
     _xlfn.XLOOKUP(
         K3,
@@ -14710,7 +14732,7 @@
 )</f>
         <v>Health Service Accessibility</v>
       </c>
-      <c r="L2" s="39" t="str" cm="1">
+      <c r="L2" s="35" t="str" cm="1">
         <f t="array" ref="L2">TRANSPOSE(
     _xlfn.XLOOKUP(
         L3,
@@ -14720,7 +14742,7 @@
 )</f>
         <v>Health Service Accessibility</v>
       </c>
-      <c r="M2" s="39" t="str" cm="1">
+      <c r="M2" s="35" t="str" cm="1">
         <f t="array" ref="M2">TRANSPOSE(
     _xlfn.XLOOKUP(
         M3,
@@ -14730,7 +14752,7 @@
 )</f>
         <v>Health Service Accessibility</v>
       </c>
-      <c r="N2" s="39" t="str" cm="1">
+      <c r="N2" s="35" t="str" cm="1">
         <f t="array" ref="N2">TRANSPOSE(
     _xlfn.XLOOKUP(
         N3,
@@ -14740,7 +14762,7 @@
 )</f>
         <v>Health Service Accessibility</v>
       </c>
-      <c r="O2" s="39" t="str" cm="1">
+      <c r="O2" s="35" t="str" cm="1">
         <f t="array" ref="O2">TRANSPOSE(
     _xlfn.XLOOKUP(
         O3,
@@ -14750,7 +14772,7 @@
 )</f>
         <v>Public Infrastructure</v>
       </c>
-      <c r="P2" s="39" t="str" cm="1">
+      <c r="P2" s="35" t="str" cm="1">
         <f t="array" ref="P2">TRANSPOSE(
     _xlfn.XLOOKUP(
         P3,
@@ -14760,7 +14782,7 @@
 )</f>
         <v>Safety and Security</v>
       </c>
-      <c r="Q2" s="39" t="str" cm="1">
+      <c r="Q2" s="35" t="str" cm="1">
         <f t="array" ref="Q2">TRANSPOSE(
     _xlfn.XLOOKUP(
         Q3,
@@ -14771,136 +14793,136 @@
         <v>Safety and Security</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="132" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
-      <c r="C3" s="40" t="str" cm="1">
+      <c r="C3" s="36" t="str" cm="1">
         <f t="array" ref="C3:Q3">TRANSPOSE(
     _xlfn._xlws.FILTER(Indicator_Metadata[Indicator],
            Indicator_Metadata[Include]=TRUE)
 )</f>
         <v>Average number of days below 10*C from October to March, Severity Score</v>
       </c>
-      <c r="D3" s="40" t="str">
+      <c r="D3" s="36" t="str">
         <v>Elderly population (60 and Above)</v>
       </c>
-      <c r="E3" s="40" t="str">
+      <c r="E3" s="36" t="str">
         <v>Infant population (Under 5)</v>
       </c>
-      <c r="F3" s="40" t="str">
+      <c r="F3" s="36" t="str">
         <v>Chronic illness (Hypertension)</v>
       </c>
-      <c r="G3" s="40" t="str">
+      <c r="G3" s="36" t="str">
         <v>Internally displaced people (IDP)</v>
       </c>
-      <c r="H3" s="40" t="str">
+      <c r="H3" s="36" t="str">
         <v>Average household income</v>
       </c>
-      <c r="I3" s="40" t="str">
+      <c r="I3" s="36" t="str">
         <v>Unable to access health services</v>
       </c>
-      <c r="J3" s="40" t="str">
+      <c r="J3" s="36" t="str">
         <v>Unable to get necessary medicine</v>
       </c>
-      <c r="K3" s="40" t="str">
+      <c r="K3" s="36" t="str">
         <v>Functioning of health facilities</v>
       </c>
-      <c r="L3" s="40" t="str">
+      <c r="L3" s="36" t="str">
         <v xml:space="preserve">Health facility power availability </v>
       </c>
-      <c r="M3" s="40" t="str">
+      <c r="M3" s="36" t="str">
         <v xml:space="preserve">Health facility heating availablity </v>
       </c>
-      <c r="N3" s="40" t="str">
+      <c r="N3" s="36" t="str">
         <v>Health cluster partner support</v>
       </c>
-      <c r="O3" s="40" t="str">
+      <c r="O3" s="36" t="str">
         <v xml:space="preserve">Frequency and duration of power outage </v>
       </c>
-      <c r="P3" s="40" t="str">
+      <c r="P3" s="36" t="str">
         <v>Attacks on healthcare  (SSA)</v>
       </c>
-      <c r="Q3" s="40" t="str">
+      <c r="Q3" s="36" t="str">
         <v>Conflict classification</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="13"/>
-      <c r="C4" s="41">
+      <c r="C4" s="37">
         <f>_xlfn.XLOOKUP(C$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>0.2</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="37">
         <f>_xlfn.XLOOKUP(D$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="37">
         <f>_xlfn.XLOOKUP(E$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="F4" s="41">
+      <c r="F4" s="37">
         <f>_xlfn.XLOOKUP(F$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="G4" s="41">
+      <c r="G4" s="37">
         <f>_xlfn.XLOOKUP(G$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="H4" s="41">
+      <c r="H4" s="37">
         <f>_xlfn.XLOOKUP(H$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="I4" s="41">
+      <c r="I4" s="37">
         <f>_xlfn.XLOOKUP(I$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="J4" s="41">
+      <c r="J4" s="37">
         <f>_xlfn.XLOOKUP(J$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="K4" s="41">
+      <c r="K4" s="37">
         <f>_xlfn.XLOOKUP(K$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L4" s="41">
+      <c r="L4" s="37">
         <f>_xlfn.XLOOKUP(L$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="M4" s="41">
+      <c r="M4" s="37">
         <f>_xlfn.XLOOKUP(M$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N4" s="41">
+      <c r="N4" s="37">
         <f>_xlfn.XLOOKUP(N$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="O4" s="41">
+      <c r="O4" s="37">
         <f>_xlfn.XLOOKUP(O$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="P4" s="41">
+      <c r="P4" s="37">
         <f>_xlfn.XLOOKUP(P$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q4" s="41">
+      <c r="Q4" s="37">
         <f>_xlfn.XLOOKUP(Q$3, 'Indicator Weights'!$A:$A, 'Indicator Weights'!$F:$F)</f>
         <v>0.1125</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="C5" s="41"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C5" s="37"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>3386</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>3385</v>
       </c>
-      <c r="C6" s="41"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C6" s="37"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="str" cm="1">
         <f t="array" ref="A7:A34">_xlfn._xlws.FILTER(Geo_Reference[Member State],Geo_Reference[ISO3]="UKR")</f>
         <v>Ukraine</v>
@@ -14909,743 +14931,744 @@
         <f t="array" ref="B7:B34">_xlfn._xlws.FILTER(Geo_Reference[Administrative Level 1], Geo_Reference[ISO3] ="UKR")</f>
         <v>Avtonomna Respublika Krym</v>
       </c>
-      <c r="C7" s="42" t="str">
+      <c r="C7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!C4), ISBLANK(C$4)), "", 'Indicator Data'!C4 * C$4)</f>
         <v/>
       </c>
-      <c r="D7" s="42" t="str">
+      <c r="D7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!D4), ISBLANK(D$4)), "", 'Indicator Data'!D4 * D$4)</f>
         <v/>
       </c>
-      <c r="E7" s="42" t="str">
+      <c r="E7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!E4), ISBLANK(E$4)), "", 'Indicator Data'!E4 * E$4)</f>
         <v/>
       </c>
-      <c r="F7" s="42" t="str">
+      <c r="F7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!F4), ISBLANK(F$4)), "", 'Indicator Data'!F4 * F$4)</f>
         <v/>
       </c>
-      <c r="G7" s="42" t="str">
+      <c r="G7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!G4), ISBLANK(G$4)), "", 'Indicator Data'!G4 * G$4)</f>
         <v/>
       </c>
-      <c r="H7" s="42" t="str">
+      <c r="H7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!H4), ISBLANK(H$4)), "", 'Indicator Data'!H4 * H$4)</f>
         <v/>
       </c>
-      <c r="I7" s="42" t="str">
+      <c r="I7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!I4), ISBLANK(I$4)), "", 'Indicator Data'!I4 * I$4)</f>
         <v/>
       </c>
-      <c r="J7" s="42" t="str">
+      <c r="J7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!J4), ISBLANK(J$4)), "", 'Indicator Data'!J4 * J$4)</f>
         <v/>
       </c>
-      <c r="K7" s="42" t="str">
+      <c r="K7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!K4), ISBLANK(K$4)), "", 'Indicator Data'!K4 * K$4)</f>
         <v/>
       </c>
-      <c r="L7" s="42" t="str">
+      <c r="L7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!L4), ISBLANK(L$4)), "", 'Indicator Data'!L4 * L$4)</f>
         <v/>
       </c>
-      <c r="M7" s="42" t="str">
+      <c r="M7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!M4), ISBLANK(M$4)), "", 'Indicator Data'!M4 * M$4)</f>
         <v/>
       </c>
-      <c r="N7" s="42" t="str">
+      <c r="N7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!N4), ISBLANK(N$4)), "", 'Indicator Data'!N4 * N$4)</f>
         <v/>
       </c>
-      <c r="O7" s="42" t="str">
+      <c r="O7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!O4), ISBLANK(O$4)), "", 'Indicator Data'!O4 * O$4)</f>
         <v/>
       </c>
-      <c r="P7" s="42" t="str">
+      <c r="P7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!P4), ISBLANK(P$4)), "", 'Indicator Data'!P4 * P$4)</f>
         <v/>
       </c>
-      <c r="Q7" s="42" t="str">
+      <c r="Q7" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!Q4), ISBLANK(Q$4)), "", 'Indicator Data'!Q4 * Q$4)</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="str">
         <v>Ukraine</v>
       </c>
       <c r="B8" s="14" t="str">
         <v>Cherkaska</v>
       </c>
-      <c r="C8" s="42">
+      <c r="C8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C5), ISBLANK(C$4)), "", 'Indicator Data'!C5 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D5), ISBLANK(D$4)), "", 'Indicator Data'!D5 * D$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="E8" s="42">
+      <c r="E8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E5), ISBLANK(E$4)), "", 'Indicator Data'!E5 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F5), ISBLANK(F$4)), "", 'Indicator Data'!F5 * F$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="G8" s="42">
+      <c r="G8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G5), ISBLANK(G$4)), "", 'Indicator Data'!G5 * G$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H8" s="42">
+      <c r="H8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H5), ISBLANK(H$4)), "", 'Indicator Data'!H5 * H$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="I8" s="42">
+      <c r="I8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I5), ISBLANK(I$4)), "", 'Indicator Data'!I5 * I$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J5), ISBLANK(J$4)), "", 'Indicator Data'!J5 * J$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="K8" s="42">
+      <c r="K8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K5), ISBLANK(K$4)), "", 'Indicator Data'!K5 * K$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="L8" s="42">
+      <c r="L8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L5), ISBLANK(L$4)), "", 'Indicator Data'!L5 * L$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="M8" s="42">
+      <c r="M8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M5), ISBLANK(M$4)), "", 'Indicator Data'!M5 * M$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="N8" s="42">
+      <c r="N8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N5), ISBLANK(N$4)), "", 'Indicator Data'!N5 * N$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="O8" s="42">
+      <c r="O8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O5), ISBLANK(O$4)), "", 'Indicator Data'!O5 * O$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="P8" s="42">
+      <c r="P8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P5), ISBLANK(P$4)), "", 'Indicator Data'!P5 * P$4)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q8" s="42">
+      <c r="Q8" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q5), ISBLANK(Q$4)), "", 'Indicator Data'!Q5 * Q$4)</f>
         <v>0.1125</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="str">
         <v>Ukraine</v>
       </c>
       <c r="B9" s="14" t="str">
         <v>Chernihivska</v>
       </c>
-      <c r="C9" s="42">
+      <c r="C9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C6), ISBLANK(C$4)), "", 'Indicator Data'!C6 * C$4)</f>
         <v>1</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D6), ISBLANK(D$4)), "", 'Indicator Data'!D6 * D$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E6), ISBLANK(E$4)), "", 'Indicator Data'!E6 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F6), ISBLANK(F$4)), "", 'Indicator Data'!F6 * F$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="G9" s="42">
+      <c r="G9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G6), ISBLANK(G$4)), "", 'Indicator Data'!G6 * G$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="H9" s="42">
+      <c r="H9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H6), ISBLANK(H$4)), "", 'Indicator Data'!H6 * H$4)</f>
         <v>0.35</v>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I6), ISBLANK(I$4)), "", 'Indicator Data'!I6 * I$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J6), ISBLANK(J$4)), "", 'Indicator Data'!J6 * J$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="K9" s="42">
+      <c r="K9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K6), ISBLANK(K$4)), "", 'Indicator Data'!K6 * K$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="L9" s="42">
+      <c r="L9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L6), ISBLANK(L$4)), "", 'Indicator Data'!L6 * L$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="M9" s="42">
+      <c r="M9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M6), ISBLANK(M$4)), "", 'Indicator Data'!M6 * M$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="N9" s="42">
+      <c r="N9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N6), ISBLANK(N$4)), "", 'Indicator Data'!N6 * N$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="O9" s="42">
+      <c r="O9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O6), ISBLANK(O$4)), "", 'Indicator Data'!O6 * O$4)</f>
         <v>0.27</v>
       </c>
-      <c r="P9" s="42">
+      <c r="P9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P6), ISBLANK(P$4)), "", 'Indicator Data'!P6 * P$4)</f>
         <v>0.33750000000000002</v>
       </c>
-      <c r="Q9" s="42">
+      <c r="Q9" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q6), ISBLANK(Q$4)), "", 'Indicator Data'!Q6 * Q$4)</f>
         <v>0.33750000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="str">
         <v>Ukraine</v>
       </c>
       <c r="B10" s="14" t="str">
         <v>Chernivetska</v>
       </c>
-      <c r="C10" s="42">
+      <c r="C10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C7), ISBLANK(C$4)), "", 'Indicator Data'!C7 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D7), ISBLANK(D$4)), "", 'Indicator Data'!D7 * D$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E7), ISBLANK(E$4)), "", 'Indicator Data'!E7 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F7), ISBLANK(F$4)), "", 'Indicator Data'!F7 * F$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="G10" s="42">
+      <c r="G10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G7), ISBLANK(G$4)), "", 'Indicator Data'!G7 * G$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="H10" s="42">
+      <c r="H10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H7), ISBLANK(H$4)), "", 'Indicator Data'!H7 * H$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I7), ISBLANK(I$4)), "", 'Indicator Data'!I7 * I$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J7), ISBLANK(J$4)), "", 'Indicator Data'!J7 * J$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="K10" s="42">
+      <c r="K10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K7), ISBLANK(K$4)), "", 'Indicator Data'!K7 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L10" s="42">
+      <c r="L10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L7), ISBLANK(L$4)), "", 'Indicator Data'!L7 * L$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="M10" s="42">
+      <c r="M10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M7), ISBLANK(M$4)), "", 'Indicator Data'!M7 * M$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="N10" s="42">
+      <c r="N10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N7), ISBLANK(N$4)), "", 'Indicator Data'!N7 * N$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="O10" s="42">
+      <c r="O10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O7), ISBLANK(O$4)), "", 'Indicator Data'!O7 * O$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="P10" s="42">
+      <c r="P10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P7), ISBLANK(P$4)), "", 'Indicator Data'!P7 * P$4)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q10" s="42">
+      <c r="Q10" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q7), ISBLANK(Q$4)), "", 'Indicator Data'!Q7 * Q$4)</f>
         <v>0.1125</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="str">
         <v>Ukraine</v>
       </c>
       <c r="B11" s="14" t="str">
         <v>Chornobylska Zona</v>
       </c>
-      <c r="C11" s="42" t="str">
+      <c r="C11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!C8), ISBLANK(C$4)), "", 'Indicator Data'!C8 * C$4)</f>
         <v/>
       </c>
-      <c r="D11" s="42" t="str">
+      <c r="D11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!D8), ISBLANK(D$4)), "", 'Indicator Data'!D8 * D$4)</f>
         <v/>
       </c>
-      <c r="E11" s="42" t="str">
+      <c r="E11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!E8), ISBLANK(E$4)), "", 'Indicator Data'!E8 * E$4)</f>
         <v/>
       </c>
-      <c r="F11" s="42" t="str">
+      <c r="F11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!F8), ISBLANK(F$4)), "", 'Indicator Data'!F8 * F$4)</f>
         <v/>
       </c>
-      <c r="G11" s="42" t="str">
+      <c r="G11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!G8), ISBLANK(G$4)), "", 'Indicator Data'!G8 * G$4)</f>
         <v/>
       </c>
-      <c r="H11" s="42" t="str">
+      <c r="H11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!H8), ISBLANK(H$4)), "", 'Indicator Data'!H8 * H$4)</f>
         <v/>
       </c>
-      <c r="I11" s="42" t="str">
+      <c r="I11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!I8), ISBLANK(I$4)), "", 'Indicator Data'!I8 * I$4)</f>
         <v/>
       </c>
-      <c r="J11" s="42" t="str">
+      <c r="J11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!J8), ISBLANK(J$4)), "", 'Indicator Data'!J8 * J$4)</f>
         <v/>
       </c>
-      <c r="K11" s="42" t="str">
+      <c r="K11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!K8), ISBLANK(K$4)), "", 'Indicator Data'!K8 * K$4)</f>
         <v/>
       </c>
-      <c r="L11" s="42" t="str">
+      <c r="L11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!L8), ISBLANK(L$4)), "", 'Indicator Data'!L8 * L$4)</f>
         <v/>
       </c>
-      <c r="M11" s="42" t="str">
+      <c r="M11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!M8), ISBLANK(M$4)), "", 'Indicator Data'!M8 * M$4)</f>
         <v/>
       </c>
-      <c r="N11" s="42" t="str">
+      <c r="N11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!N8), ISBLANK(N$4)), "", 'Indicator Data'!N8 * N$4)</f>
         <v/>
       </c>
-      <c r="O11" s="42" t="str">
+      <c r="O11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!O8), ISBLANK(O$4)), "", 'Indicator Data'!O8 * O$4)</f>
         <v/>
       </c>
-      <c r="P11" s="42" t="str">
+      <c r="P11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!P8), ISBLANK(P$4)), "", 'Indicator Data'!P8 * P$4)</f>
         <v/>
       </c>
-      <c r="Q11" s="42" t="str">
+      <c r="Q11" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!Q8), ISBLANK(Q$4)), "", 'Indicator Data'!Q8 * Q$4)</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="str">
         <v>Ukraine</v>
       </c>
       <c r="B12" s="14" t="str">
         <v>Dnipropetrovska</v>
       </c>
-      <c r="C12" s="42">
+      <c r="C12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C9), ISBLANK(C$4)), "", 'Indicator Data'!C9 * C$4)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D9), ISBLANK(D$4)), "", 'Indicator Data'!D9 * D$4)</f>
         <v>0.35</v>
       </c>
-      <c r="E12" s="42">
+      <c r="E12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E9), ISBLANK(E$4)), "", 'Indicator Data'!E9 * E$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F9), ISBLANK(F$4)), "", 'Indicator Data'!F9 * F$4)</f>
         <v>0.35</v>
       </c>
-      <c r="G12" s="42">
+      <c r="G12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G9), ISBLANK(G$4)), "", 'Indicator Data'!G9 * G$4)</f>
         <v>0.35</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H9), ISBLANK(H$4)), "", 'Indicator Data'!H9 * H$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I9), ISBLANK(I$4)), "", 'Indicator Data'!I9 * I$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="J12" s="42">
+      <c r="J12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J9), ISBLANK(J$4)), "", 'Indicator Data'!J9 * J$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="K12" s="42">
+      <c r="K12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K9), ISBLANK(K$4)), "", 'Indicator Data'!K9 * K$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="L12" s="42">
+      <c r="L12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L9), ISBLANK(L$4)), "", 'Indicator Data'!L9 * L$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="M12" s="42">
+      <c r="M12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M9), ISBLANK(M$4)), "", 'Indicator Data'!M9 * M$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="N12" s="42">
+      <c r="N12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N9), ISBLANK(N$4)), "", 'Indicator Data'!N9 * N$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="O12" s="42">
+      <c r="O12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O9), ISBLANK(O$4)), "", 'Indicator Data'!O9 * O$4)</f>
         <v>0.36000000000000004</v>
       </c>
-      <c r="P12" s="42">
+      <c r="P12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P9), ISBLANK(P$4)), "", 'Indicator Data'!P9 * P$4)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q12" s="42">
+      <c r="Q12" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q9), ISBLANK(Q$4)), "", 'Indicator Data'!Q9 * Q$4)</f>
         <v>0.33750000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="str">
         <v>Ukraine</v>
       </c>
       <c r="B13" s="14" t="str">
         <v>Donetska</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C10), ISBLANK(C$4)), "", 'Indicator Data'!C10 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D10), ISBLANK(D$4)), "", 'Indicator Data'!D10 * D$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E10), ISBLANK(E$4)), "", 'Indicator Data'!E10 * E$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F10), ISBLANK(F$4)), "", 'Indicator Data'!F10 * F$4)</f>
         <v>0.35</v>
       </c>
-      <c r="G13" s="42">
+      <c r="G13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G10), ISBLANK(G$4)), "", 'Indicator Data'!G10 * G$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="H13" s="42" t="str">
+      <c r="H13" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!H10), ISBLANK(H$4)), "", 'Indicator Data'!H10 * H$4)</f>
         <v/>
       </c>
-      <c r="I13" s="42">
+      <c r="I13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I10), ISBLANK(I$4)), "", 'Indicator Data'!I10 * I$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="J13" s="42">
+      <c r="J13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J10), ISBLANK(J$4)), "", 'Indicator Data'!J10 * J$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="K13" s="42">
+      <c r="K13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K10), ISBLANK(K$4)), "", 'Indicator Data'!K10 * K$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="L13" s="42">
+      <c r="L13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L10), ISBLANK(L$4)), "", 'Indicator Data'!L10 * L$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="M13" s="42">
+      <c r="M13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M10), ISBLANK(M$4)), "", 'Indicator Data'!M10 * M$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="N13" s="42">
+      <c r="N13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N10), ISBLANK(N$4)), "", 'Indicator Data'!N10 * N$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="O13" s="42">
+      <c r="O13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O10), ISBLANK(O$4)), "", 'Indicator Data'!O10 * O$4)</f>
         <v>0.45000000000000007</v>
       </c>
-      <c r="P13" s="42">
+      <c r="P13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P10), ISBLANK(P$4)), "", 'Indicator Data'!P10 * P$4)</f>
         <v>0.5625</v>
       </c>
-      <c r="Q13" s="42">
+      <c r="Q13" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q10), ISBLANK(Q$4)), "", 'Indicator Data'!Q10 * Q$4)</f>
         <v>0.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="str">
         <v>Ukraine</v>
       </c>
       <c r="B14" s="14" t="str">
         <v>Ivano-Frankivska</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C11), ISBLANK(C$4)), "", 'Indicator Data'!C11 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D11), ISBLANK(D$4)), "", 'Indicator Data'!D11 * D$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E14" s="42">
+      <c r="E14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E11), ISBLANK(E$4)), "", 'Indicator Data'!E11 * E$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="F14" s="42">
+      <c r="F14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F11), ISBLANK(F$4)), "", 'Indicator Data'!F11 * F$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="G14" s="42">
+      <c r="G14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G11), ISBLANK(G$4)), "", 'Indicator Data'!G11 * G$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="H14" s="42">
+      <c r="H14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H11), ISBLANK(H$4)), "", 'Indicator Data'!H11 * H$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="I14" s="42">
+      <c r="I14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I11), ISBLANK(I$4)), "", 'Indicator Data'!I11 * I$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="J14" s="42">
+      <c r="J14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J11), ISBLANK(J$4)), "", 'Indicator Data'!J11 * J$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="K14" s="42">
+      <c r="K14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K11), ISBLANK(K$4)), "", 'Indicator Data'!K11 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L14" s="42">
+      <c r="L14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L11), ISBLANK(L$4)), "", 'Indicator Data'!L11 * L$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="M14" s="42">
+      <c r="M14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M11), ISBLANK(M$4)), "", 'Indicator Data'!M11 * M$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N14" s="42">
+      <c r="N14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N11), ISBLANK(N$4)), "", 'Indicator Data'!N11 * N$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="O14" s="42">
+      <c r="O14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O11), ISBLANK(O$4)), "", 'Indicator Data'!O11 * O$4)</f>
         <v>0.36000000000000004</v>
       </c>
-      <c r="P14" s="42">
+      <c r="P14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P11), ISBLANK(P$4)), "", 'Indicator Data'!P11 * P$4)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q14" s="42">
+      <c r="Q14" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q11), ISBLANK(Q$4)), "", 'Indicator Data'!Q11 * Q$4)</f>
         <v>0.1125</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="str">
         <v>Ukraine</v>
       </c>
       <c r="B15" s="14" t="str">
         <v>Kharkivska</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C12), ISBLANK(C$4)), "", 'Indicator Data'!C12 * C$4)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D12), ISBLANK(D$4)), "", 'Indicator Data'!D12 * D$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="E15" s="42">
+      <c r="E15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E12), ISBLANK(E$4)), "", 'Indicator Data'!E12 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F15" s="42">
+      <c r="F15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F12), ISBLANK(F$4)), "", 'Indicator Data'!F12 * F$4)</f>
         <v>0.35</v>
       </c>
-      <c r="G15" s="42">
+      <c r="G15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G12), ISBLANK(G$4)), "", 'Indicator Data'!G12 * G$4)</f>
         <v>0.35</v>
       </c>
-      <c r="H15" s="42">
+      <c r="H15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H12), ISBLANK(H$4)), "", 'Indicator Data'!H12 * H$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="I15" s="42">
+      <c r="I15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I12), ISBLANK(I$4)), "", 'Indicator Data'!I12 * I$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="J15" s="42">
+      <c r="J15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J12), ISBLANK(J$4)), "", 'Indicator Data'!J12 * J$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="K15" s="42">
+      <c r="K15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K12), ISBLANK(K$4)), "", 'Indicator Data'!K12 * K$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="L15" s="42">
+      <c r="L15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L12), ISBLANK(L$4)), "", 'Indicator Data'!L12 * L$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="M15" s="42">
+      <c r="M15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M12), ISBLANK(M$4)), "", 'Indicator Data'!M12 * M$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="N15" s="42">
+      <c r="N15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N12), ISBLANK(N$4)), "", 'Indicator Data'!N12 * N$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="O15" s="42">
+      <c r="O15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O12), ISBLANK(O$4)), "", 'Indicator Data'!O12 * O$4)</f>
         <v>0.36000000000000004</v>
       </c>
-      <c r="P15" s="42">
+      <c r="P15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P12), ISBLANK(P$4)), "", 'Indicator Data'!P12 * P$4)</f>
         <v>0.5625</v>
       </c>
-      <c r="Q15" s="42">
+      <c r="Q15" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q12), ISBLANK(Q$4)), "", 'Indicator Data'!Q12 * Q$4)</f>
         <v>0.5625</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="str">
         <v>Ukraine</v>
       </c>
       <c r="B16" s="14" t="str">
         <v>Khersonska</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C13), ISBLANK(C$4)), "", 'Indicator Data'!C13 * C$4)</f>
         <v>0.4</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D13), ISBLANK(D$4)), "", 'Indicator Data'!D13 * D$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="E16" s="42">
+      <c r="E16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E13), ISBLANK(E$4)), "", 'Indicator Data'!E13 * E$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F13), ISBLANK(F$4)), "", 'Indicator Data'!F13 * F$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="G16" s="42">
+      <c r="G16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G13), ISBLANK(G$4)), "", 'Indicator Data'!G13 * G$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="H16" s="42" t="str">
+      <c r="H16" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!H13), ISBLANK(H$4)), "", 'Indicator Data'!H13 * H$4)</f>
         <v/>
       </c>
-      <c r="I16" s="42">
+      <c r="I16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I13), ISBLANK(I$4)), "", 'Indicator Data'!I13 * I$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="J16" s="42">
+      <c r="J16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J13), ISBLANK(J$4)), "", 'Indicator Data'!J13 * J$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="K16" s="42">
+      <c r="K16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K13), ISBLANK(K$4)), "", 'Indicator Data'!K13 * K$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="L16" s="42">
+      <c r="L16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L13), ISBLANK(L$4)), "", 'Indicator Data'!L13 * L$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="M16" s="42">
+      <c r="M16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M13), ISBLANK(M$4)), "", 'Indicator Data'!M13 * M$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="N16" s="42">
+      <c r="N16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N13), ISBLANK(N$4)), "", 'Indicator Data'!N13 * N$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="O16" s="42">
+      <c r="O16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O13), ISBLANK(O$4)), "", 'Indicator Data'!O13 * O$4)</f>
         <v>0.45000000000000007</v>
       </c>
-      <c r="P16" s="42">
+      <c r="P16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P13), ISBLANK(P$4)), "", 'Indicator Data'!P13 * P$4)</f>
         <v>0.5625</v>
       </c>
-      <c r="Q16" s="42">
+      <c r="Q16" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q13), ISBLANK(Q$4)), "", 'Indicator Data'!Q13 * Q$4)</f>
         <v>0.5625</v>
       </c>
+      <c r="T16" s="44"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="str">
         <v>Ukraine</v>
       </c>
-      <c r="B17" s="43" t="str">
+      <c r="B17" s="39" t="str">
         <v>Khmelnytska</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C14), ISBLANK(C$4)), "", 'Indicator Data'!C14 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D14), ISBLANK(D$4)), "", 'Indicator Data'!D14 * D$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="E17" s="42">
+      <c r="E17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E14), ISBLANK(E$4)), "", 'Indicator Data'!E14 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F14), ISBLANK(F$4)), "", 'Indicator Data'!F14 * F$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="G17" s="42">
+      <c r="G17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G14), ISBLANK(G$4)), "", 'Indicator Data'!G14 * G$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="H17" s="42">
+      <c r="H17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H14), ISBLANK(H$4)), "", 'Indicator Data'!H14 * H$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="I17" s="42">
+      <c r="I17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I14), ISBLANK(I$4)), "", 'Indicator Data'!I14 * I$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="J17" s="42">
+      <c r="J17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J14), ISBLANK(J$4)), "", 'Indicator Data'!J14 * J$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="K17" s="42">
+      <c r="K17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K14), ISBLANK(K$4)), "", 'Indicator Data'!K14 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L17" s="42">
+      <c r="L17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L14), ISBLANK(L$4)), "", 'Indicator Data'!L14 * L$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="M17" s="42">
+      <c r="M17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M14), ISBLANK(M$4)), "", 'Indicator Data'!M14 * M$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N17" s="42">
+      <c r="N17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N14), ISBLANK(N$4)), "", 'Indicator Data'!N14 * N$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="O17" s="42">
+      <c r="O17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O14), ISBLANK(O$4)), "", 'Indicator Data'!O14 * O$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="P17" s="42">
+      <c r="P17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P14), ISBLANK(P$4)), "", 'Indicator Data'!P14 * P$4)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q17" s="42">
+      <c r="Q17" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q14), ISBLANK(Q$4)), "", 'Indicator Data'!Q14 * Q$4)</f>
         <v>0.1125</v>
       </c>
@@ -15657,63 +15680,63 @@
       <c r="B18" s="14" t="str">
         <v>Kirovohradska</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C15), ISBLANK(C$4)), "", 'Indicator Data'!C15 * C$4)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D15), ISBLANK(D$4)), "", 'Indicator Data'!D15 * D$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E18" s="42">
+      <c r="E18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E15), ISBLANK(E$4)), "", 'Indicator Data'!E15 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F18" s="42">
+      <c r="F18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F15), ISBLANK(F$4)), "", 'Indicator Data'!F15 * F$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="G18" s="42">
+      <c r="G18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G15), ISBLANK(G$4)), "", 'Indicator Data'!G15 * G$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="H18" s="42">
+      <c r="H18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H15), ISBLANK(H$4)), "", 'Indicator Data'!H15 * H$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="I18" s="42">
+      <c r="I18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I15), ISBLANK(I$4)), "", 'Indicator Data'!I15 * I$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="J18" s="42">
+      <c r="J18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J15), ISBLANK(J$4)), "", 'Indicator Data'!J15 * J$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="K18" s="42">
+      <c r="K18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K15), ISBLANK(K$4)), "", 'Indicator Data'!K15 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L18" s="42">
+      <c r="L18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L15), ISBLANK(L$4)), "", 'Indicator Data'!L15 * L$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="M18" s="42">
+      <c r="M18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M15), ISBLANK(M$4)), "", 'Indicator Data'!M15 * M$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N18" s="42">
+      <c r="N18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N15), ISBLANK(N$4)), "", 'Indicator Data'!N15 * N$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="O18" s="42">
+      <c r="O18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O15), ISBLANK(O$4)), "", 'Indicator Data'!O15 * O$4)</f>
         <v>0.36000000000000004</v>
       </c>
-      <c r="P18" s="42">
+      <c r="P18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P15), ISBLANK(P$4)), "", 'Indicator Data'!P15 * P$4)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q18" s="42">
+      <c r="Q18" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q15), ISBLANK(Q$4)), "", 'Indicator Data'!Q15 * Q$4)</f>
         <v>0.1125</v>
       </c>
@@ -15725,63 +15748,63 @@
       <c r="B19" s="14" t="str">
         <v>Kyivska</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C16), ISBLANK(C$4)), "", 'Indicator Data'!C16 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D16), ISBLANK(D$4)), "", 'Indicator Data'!D16 * D$4)</f>
         <v>0.35</v>
       </c>
-      <c r="E19" s="42">
+      <c r="E19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E16), ISBLANK(E$4)), "", 'Indicator Data'!E16 * E$4)</f>
         <v>0.35</v>
       </c>
-      <c r="F19" s="42">
+      <c r="F19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F16), ISBLANK(F$4)), "", 'Indicator Data'!F16 * F$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="G19" s="42">
+      <c r="G19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G16), ISBLANK(G$4)), "", 'Indicator Data'!G16 * G$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H19" s="42">
+      <c r="H19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H16), ISBLANK(H$4)), "", 'Indicator Data'!H16 * H$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="I19" s="42">
+      <c r="I19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I16), ISBLANK(I$4)), "", 'Indicator Data'!I16 * I$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="J19" s="42">
+      <c r="J19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J16), ISBLANK(J$4)), "", 'Indicator Data'!J16 * J$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="K19" s="42">
+      <c r="K19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K16), ISBLANK(K$4)), "", 'Indicator Data'!K16 * K$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="L19" s="42">
+      <c r="L19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L16), ISBLANK(L$4)), "", 'Indicator Data'!L16 * L$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="M19" s="42">
+      <c r="M19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M16), ISBLANK(M$4)), "", 'Indicator Data'!M16 * M$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N19" s="42">
+      <c r="N19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N16), ISBLANK(N$4)), "", 'Indicator Data'!N16 * N$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="O19" s="42">
+      <c r="O19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O16), ISBLANK(O$4)), "", 'Indicator Data'!O16 * O$4)</f>
         <v>0.27</v>
       </c>
-      <c r="P19" s="42">
+      <c r="P19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P16), ISBLANK(P$4)), "", 'Indicator Data'!P16 * P$4)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q19" s="42">
+      <c r="Q19" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q16), ISBLANK(Q$4)), "", 'Indicator Data'!Q16 * Q$4)</f>
         <v>0.33750000000000002</v>
       </c>
@@ -15793,63 +15816,63 @@
       <c r="B20" s="14" t="str">
         <v>Luhanska</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!C17), ISBLANK(C$4)), "", 'Indicator Data'!C17 * C$4)</f>
-        <v>1</v>
-      </c>
-      <c r="D20" s="42">
+        <v/>
+      </c>
+      <c r="D20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!D17), ISBLANK(D$4)), "", 'Indicator Data'!D17 * D$4)</f>
-        <v>0.13999999999999999</v>
-      </c>
-      <c r="E20" s="42">
+        <v/>
+      </c>
+      <c r="E20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!E17), ISBLANK(E$4)), "", 'Indicator Data'!E17 * E$4)</f>
-        <v>6.9999999999999993E-2</v>
-      </c>
-      <c r="F20" s="42">
+        <v/>
+      </c>
+      <c r="F20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!F17), ISBLANK(F$4)), "", 'Indicator Data'!F17 * F$4)</f>
-        <v>0.35</v>
-      </c>
-      <c r="G20" s="42" t="str">
+        <v/>
+      </c>
+      <c r="G20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!G17), ISBLANK(G$4)), "", 'Indicator Data'!G17 * G$4)</f>
         <v/>
       </c>
-      <c r="H20" s="42" t="str">
+      <c r="H20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!H17), ISBLANK(H$4)), "", 'Indicator Data'!H17 * H$4)</f>
         <v/>
       </c>
-      <c r="I20" s="42" t="str">
+      <c r="I20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!I17), ISBLANK(I$4)), "", 'Indicator Data'!I17 * I$4)</f>
         <v/>
       </c>
-      <c r="J20" s="42" t="str">
+      <c r="J20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!J17), ISBLANK(J$4)), "", 'Indicator Data'!J17 * J$4)</f>
         <v/>
       </c>
-      <c r="K20" s="42" t="str">
+      <c r="K20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!K17), ISBLANK(K$4)), "", 'Indicator Data'!K17 * K$4)</f>
         <v/>
       </c>
-      <c r="L20" s="42" t="str">
+      <c r="L20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!L17), ISBLANK(L$4)), "", 'Indicator Data'!L17 * L$4)</f>
         <v/>
       </c>
-      <c r="M20" s="42" t="str">
+      <c r="M20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!M17), ISBLANK(M$4)), "", 'Indicator Data'!M17 * M$4)</f>
         <v/>
       </c>
-      <c r="N20" s="42">
+      <c r="N20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!N17), ISBLANK(N$4)), "", 'Indicator Data'!N17 * N$4)</f>
-        <v>0.11250000000000002</v>
-      </c>
-      <c r="O20" s="42">
+        <v/>
+      </c>
+      <c r="O20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!O17), ISBLANK(O$4)), "", 'Indicator Data'!O17 * O$4)</f>
-        <v>0.45000000000000007</v>
-      </c>
-      <c r="P20" s="42">
+        <v/>
+      </c>
+      <c r="P20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!P17), ISBLANK(P$4)), "", 'Indicator Data'!P17 * P$4)</f>
-        <v>0.33750000000000002</v>
-      </c>
-      <c r="Q20" s="42" t="str">
+        <v/>
+      </c>
+      <c r="Q20" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!Q17), ISBLANK(Q$4)), "", 'Indicator Data'!Q17 * Q$4)</f>
         <v/>
       </c>
@@ -15861,63 +15884,63 @@
       <c r="B21" s="14" t="str">
         <v>Lvivska</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C18), ISBLANK(C$4)), "", 'Indicator Data'!C18 * C$4)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D18), ISBLANK(D$4)), "", 'Indicator Data'!D18 * D$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="E21" s="42">
+      <c r="E21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E18), ISBLANK(E$4)), "", 'Indicator Data'!E18 * E$4)</f>
         <v>0.35</v>
       </c>
-      <c r="F21" s="42">
+      <c r="F21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F18), ISBLANK(F$4)), "", 'Indicator Data'!F18 * F$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="G21" s="42">
+      <c r="G21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G18), ISBLANK(G$4)), "", 'Indicator Data'!G18 * G$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H21" s="42">
+      <c r="H21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H18), ISBLANK(H$4)), "", 'Indicator Data'!H18 * H$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="I21" s="42">
+      <c r="I21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I18), ISBLANK(I$4)), "", 'Indicator Data'!I18 * I$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="J21" s="42">
+      <c r="J21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J18), ISBLANK(J$4)), "", 'Indicator Data'!J18 * J$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="K21" s="42">
+      <c r="K21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K18), ISBLANK(K$4)), "", 'Indicator Data'!K18 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L21" s="42">
+      <c r="L21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L18), ISBLANK(L$4)), "", 'Indicator Data'!L18 * L$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="M21" s="42">
+      <c r="M21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M18), ISBLANK(M$4)), "", 'Indicator Data'!M18 * M$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N21" s="42">
+      <c r="N21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N18), ISBLANK(N$4)), "", 'Indicator Data'!N18 * N$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="O21" s="42">
+      <c r="O21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O18), ISBLANK(O$4)), "", 'Indicator Data'!O18 * O$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="P21" s="42">
+      <c r="P21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P18), ISBLANK(P$4)), "", 'Indicator Data'!P18 * P$4)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q21" s="42">
+      <c r="Q21" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q18), ISBLANK(Q$4)), "", 'Indicator Data'!Q18 * Q$4)</f>
         <v>0.1125</v>
       </c>
@@ -15929,63 +15952,63 @@
       <c r="B22" s="14" t="str">
         <v>Misto Kyiv</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C19), ISBLANK(C$4)), "", 'Indicator Data'!C19 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D22" s="42">
+      <c r="D22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D19), ISBLANK(D$4)), "", 'Indicator Data'!D19 * D$4)</f>
         <v>0.35</v>
       </c>
-      <c r="E22" s="42">
+      <c r="E22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E19), ISBLANK(E$4)), "", 'Indicator Data'!E19 * E$4)</f>
         <v>0.35</v>
       </c>
-      <c r="F22" s="42">
+      <c r="F22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F19), ISBLANK(F$4)), "", 'Indicator Data'!F19 * F$4)</f>
         <v>0.35</v>
       </c>
-      <c r="G22" s="42">
+      <c r="G22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G19), ISBLANK(G$4)), "", 'Indicator Data'!G19 * G$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H22" s="42">
+      <c r="H22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H19), ISBLANK(H$4)), "", 'Indicator Data'!H19 * H$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="I22" s="42">
+      <c r="I22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I19), ISBLANK(I$4)), "", 'Indicator Data'!I19 * I$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="J22" s="42">
+      <c r="J22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J19), ISBLANK(J$4)), "", 'Indicator Data'!J19 * J$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="K22" s="42">
+      <c r="K22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K19), ISBLANK(K$4)), "", 'Indicator Data'!K19 * K$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="L22" s="42">
+      <c r="L22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L19), ISBLANK(L$4)), "", 'Indicator Data'!L19 * L$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="M22" s="42">
+      <c r="M22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M19), ISBLANK(M$4)), "", 'Indicator Data'!M19 * M$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="N22" s="42">
+      <c r="N22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N19), ISBLANK(N$4)), "", 'Indicator Data'!N19 * N$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="O22" s="42">
+      <c r="O22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O19), ISBLANK(O$4)), "", 'Indicator Data'!O19 * O$4)</f>
         <v>0.27</v>
       </c>
-      <c r="P22" s="42">
+      <c r="P22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P19), ISBLANK(P$4)), "", 'Indicator Data'!P19 * P$4)</f>
         <v>0.45</v>
       </c>
-      <c r="Q22" s="42">
+      <c r="Q22" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q19), ISBLANK(Q$4)), "", 'Indicator Data'!Q19 * Q$4)</f>
         <v>0.33750000000000002</v>
       </c>
@@ -15997,63 +16020,63 @@
       <c r="B23" s="14" t="str">
         <v>Misto Sevastopol</v>
       </c>
-      <c r="C23" s="42" t="str">
+      <c r="C23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!C20), ISBLANK(C$4)), "", 'Indicator Data'!C20 * C$4)</f>
         <v/>
       </c>
-      <c r="D23" s="42" t="str">
+      <c r="D23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!D20), ISBLANK(D$4)), "", 'Indicator Data'!D20 * D$4)</f>
         <v/>
       </c>
-      <c r="E23" s="42" t="str">
+      <c r="E23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!E20), ISBLANK(E$4)), "", 'Indicator Data'!E20 * E$4)</f>
         <v/>
       </c>
-      <c r="F23" s="42" t="str">
+      <c r="F23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!F20), ISBLANK(F$4)), "", 'Indicator Data'!F20 * F$4)</f>
         <v/>
       </c>
-      <c r="G23" s="42" t="str">
+      <c r="G23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!G20), ISBLANK(G$4)), "", 'Indicator Data'!G20 * G$4)</f>
         <v/>
       </c>
-      <c r="H23" s="42" t="str">
+      <c r="H23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!H20), ISBLANK(H$4)), "", 'Indicator Data'!H20 * H$4)</f>
         <v/>
       </c>
-      <c r="I23" s="42" t="str">
+      <c r="I23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!I20), ISBLANK(I$4)), "", 'Indicator Data'!I20 * I$4)</f>
         <v/>
       </c>
-      <c r="J23" s="42" t="str">
+      <c r="J23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!J20), ISBLANK(J$4)), "", 'Indicator Data'!J20 * J$4)</f>
         <v/>
       </c>
-      <c r="K23" s="42" t="str">
+      <c r="K23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!K20), ISBLANK(K$4)), "", 'Indicator Data'!K20 * K$4)</f>
         <v/>
       </c>
-      <c r="L23" s="42" t="str">
+      <c r="L23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!L20), ISBLANK(L$4)), "", 'Indicator Data'!L20 * L$4)</f>
         <v/>
       </c>
-      <c r="M23" s="42" t="str">
+      <c r="M23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!M20), ISBLANK(M$4)), "", 'Indicator Data'!M20 * M$4)</f>
         <v/>
       </c>
-      <c r="N23" s="42" t="str">
+      <c r="N23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!N20), ISBLANK(N$4)), "", 'Indicator Data'!N20 * N$4)</f>
         <v/>
       </c>
-      <c r="O23" s="42" t="str">
+      <c r="O23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!O20), ISBLANK(O$4)), "", 'Indicator Data'!O20 * O$4)</f>
         <v/>
       </c>
-      <c r="P23" s="42" t="str">
+      <c r="P23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!P20), ISBLANK(P$4)), "", 'Indicator Data'!P20 * P$4)</f>
         <v/>
       </c>
-      <c r="Q23" s="42" t="str">
+      <c r="Q23" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!Q20), ISBLANK(Q$4)), "", 'Indicator Data'!Q20 * Q$4)</f>
         <v/>
       </c>
@@ -16065,63 +16088,63 @@
       <c r="B24" s="14" t="str">
         <v>Mykolaivska</v>
       </c>
-      <c r="C24" s="42">
+      <c r="C24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C21), ISBLANK(C$4)), "", 'Indicator Data'!C21 * C$4)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D21), ISBLANK(D$4)), "", 'Indicator Data'!D21 * D$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E24" s="42">
+      <c r="E24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E21), ISBLANK(E$4)), "", 'Indicator Data'!E21 * E$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="F24" s="42">
+      <c r="F24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F21), ISBLANK(F$4)), "", 'Indicator Data'!F21 * F$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="G24" s="42">
+      <c r="G24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G21), ISBLANK(G$4)), "", 'Indicator Data'!G21 * G$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="H24" s="42">
+      <c r="H24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H21), ISBLANK(H$4)), "", 'Indicator Data'!H21 * H$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="I24" s="42">
+      <c r="I24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I21), ISBLANK(I$4)), "", 'Indicator Data'!I21 * I$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="J24" s="42">
+      <c r="J24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J21), ISBLANK(J$4)), "", 'Indicator Data'!J21 * J$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="K24" s="42">
+      <c r="K24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K21), ISBLANK(K$4)), "", 'Indicator Data'!K21 * K$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="L24" s="42">
+      <c r="L24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L21), ISBLANK(L$4)), "", 'Indicator Data'!L21 * L$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="M24" s="42">
+      <c r="M24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M21), ISBLANK(M$4)), "", 'Indicator Data'!M21 * M$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="N24" s="42">
+      <c r="N24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N21), ISBLANK(N$4)), "", 'Indicator Data'!N21 * N$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="O24" s="42">
+      <c r="O24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O21), ISBLANK(O$4)), "", 'Indicator Data'!O21 * O$4)</f>
         <v>0.36000000000000004</v>
       </c>
-      <c r="P24" s="42">
+      <c r="P24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P21), ISBLANK(P$4)), "", 'Indicator Data'!P21 * P$4)</f>
         <v>0.45</v>
       </c>
-      <c r="Q24" s="42">
+      <c r="Q24" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q21), ISBLANK(Q$4)), "", 'Indicator Data'!Q21 * Q$4)</f>
         <v>0.33750000000000002</v>
       </c>
@@ -16133,63 +16156,63 @@
       <c r="B25" s="14" t="str">
         <v>Odeska</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C22), ISBLANK(C$4)), "", 'Indicator Data'!C22 * C$4)</f>
         <v>0.4</v>
       </c>
-      <c r="D25" s="42">
+      <c r="D25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D22), ISBLANK(D$4)), "", 'Indicator Data'!D22 * D$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="E25" s="42">
+      <c r="E25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E22), ISBLANK(E$4)), "", 'Indicator Data'!E22 * E$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="F25" s="42">
+      <c r="F25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F22), ISBLANK(F$4)), "", 'Indicator Data'!F22 * F$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="G25" s="42">
+      <c r="G25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G22), ISBLANK(G$4)), "", 'Indicator Data'!G22 * G$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H25" s="42">
+      <c r="H25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H22), ISBLANK(H$4)), "", 'Indicator Data'!H22 * H$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="I25" s="42">
+      <c r="I25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I22), ISBLANK(I$4)), "", 'Indicator Data'!I22 * I$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="J25" s="42">
+      <c r="J25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J22), ISBLANK(J$4)), "", 'Indicator Data'!J22 * J$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="K25" s="42">
+      <c r="K25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K22), ISBLANK(K$4)), "", 'Indicator Data'!K22 * K$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="L25" s="42">
+      <c r="L25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L22), ISBLANK(L$4)), "", 'Indicator Data'!L22 * L$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="M25" s="42">
+      <c r="M25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M22), ISBLANK(M$4)), "", 'Indicator Data'!M22 * M$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="N25" s="42">
+      <c r="N25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N22), ISBLANK(N$4)), "", 'Indicator Data'!N22 * N$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="O25" s="42">
+      <c r="O25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O22), ISBLANK(O$4)), "", 'Indicator Data'!O22 * O$4)</f>
         <v>0.36000000000000004</v>
       </c>
-      <c r="P25" s="42">
+      <c r="P25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P22), ISBLANK(P$4)), "", 'Indicator Data'!P22 * P$4)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q25" s="42">
+      <c r="Q25" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q22), ISBLANK(Q$4)), "", 'Indicator Data'!Q22 * Q$4)</f>
         <v>0.33750000000000002</v>
       </c>
@@ -16201,63 +16224,63 @@
       <c r="B26" s="14" t="str">
         <v>Poltavska</v>
       </c>
-      <c r="C26" s="42">
+      <c r="C26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C23), ISBLANK(C$4)), "", 'Indicator Data'!C23 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D23), ISBLANK(D$4)), "", 'Indicator Data'!D23 * D$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="E26" s="42">
+      <c r="E26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E23), ISBLANK(E$4)), "", 'Indicator Data'!E23 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F26" s="42">
+      <c r="F26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F23), ISBLANK(F$4)), "", 'Indicator Data'!F23 * F$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="G26" s="42">
+      <c r="G26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G23), ISBLANK(G$4)), "", 'Indicator Data'!G23 * G$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H26" s="42">
+      <c r="H26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H23), ISBLANK(H$4)), "", 'Indicator Data'!H23 * H$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="I26" s="42">
+      <c r="I26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I23), ISBLANK(I$4)), "", 'Indicator Data'!I23 * I$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="J26" s="42">
+      <c r="J26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J23), ISBLANK(J$4)), "", 'Indicator Data'!J23 * J$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="K26" s="42">
+      <c r="K26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K23), ISBLANK(K$4)), "", 'Indicator Data'!K23 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L26" s="42">
+      <c r="L26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L23), ISBLANK(L$4)), "", 'Indicator Data'!L23 * L$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="M26" s="42">
+      <c r="M26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M23), ISBLANK(M$4)), "", 'Indicator Data'!M23 * M$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="N26" s="42">
+      <c r="N26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N23), ISBLANK(N$4)), "", 'Indicator Data'!N23 * N$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="O26" s="42">
+      <c r="O26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O23), ISBLANK(O$4)), "", 'Indicator Data'!O23 * O$4)</f>
         <v>0.27</v>
       </c>
-      <c r="P26" s="42">
+      <c r="P26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P23), ISBLANK(P$4)), "", 'Indicator Data'!P23 * P$4)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q26" s="42">
+      <c r="Q26" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q23), ISBLANK(Q$4)), "", 'Indicator Data'!Q23 * Q$4)</f>
         <v>0.1125</v>
       </c>
@@ -16269,63 +16292,63 @@
       <c r="B27" s="14" t="str">
         <v>Rivnenska</v>
       </c>
-      <c r="C27" s="42">
+      <c r="C27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C24), ISBLANK(C$4)), "", 'Indicator Data'!C24 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D24), ISBLANK(D$4)), "", 'Indicator Data'!D24 * D$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E24), ISBLANK(E$4)), "", 'Indicator Data'!E24 * E$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="F27" s="42">
+      <c r="F27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F24), ISBLANK(F$4)), "", 'Indicator Data'!F24 * F$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="G27" s="42">
+      <c r="G27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G24), ISBLANK(G$4)), "", 'Indicator Data'!G24 * G$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="H27" s="42">
+      <c r="H27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H24), ISBLANK(H$4)), "", 'Indicator Data'!H24 * H$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="I27" s="42">
+      <c r="I27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I24), ISBLANK(I$4)), "", 'Indicator Data'!I24 * I$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="J27" s="42">
+      <c r="J27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J24), ISBLANK(J$4)), "", 'Indicator Data'!J24 * J$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="K27" s="42">
+      <c r="K27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K24), ISBLANK(K$4)), "", 'Indicator Data'!K24 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L27" s="42">
+      <c r="L27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L24), ISBLANK(L$4)), "", 'Indicator Data'!L24 * L$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="M27" s="42">
+      <c r="M27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M24), ISBLANK(M$4)), "", 'Indicator Data'!M24 * M$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N27" s="42">
+      <c r="N27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N24), ISBLANK(N$4)), "", 'Indicator Data'!N24 * N$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="O27" s="42">
+      <c r="O27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O24), ISBLANK(O$4)), "", 'Indicator Data'!O24 * O$4)</f>
         <v>0.27</v>
       </c>
-      <c r="P27" s="42">
+      <c r="P27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P24), ISBLANK(P$4)), "", 'Indicator Data'!P24 * P$4)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q27" s="42">
+      <c r="Q27" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q24), ISBLANK(Q$4)), "", 'Indicator Data'!Q24 * Q$4)</f>
         <v>0.1125</v>
       </c>
@@ -16337,63 +16360,63 @@
       <c r="B28" s="14" t="str">
         <v>Sumska</v>
       </c>
-      <c r="C28" s="42">
+      <c r="C28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C25), ISBLANK(C$4)), "", 'Indicator Data'!C25 * C$4)</f>
         <v>1</v>
       </c>
-      <c r="D28" s="42">
+      <c r="D28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D25), ISBLANK(D$4)), "", 'Indicator Data'!D25 * D$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E28" s="42">
+      <c r="E28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E25), ISBLANK(E$4)), "", 'Indicator Data'!E25 * E$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="F28" s="42">
+      <c r="F28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F25), ISBLANK(F$4)), "", 'Indicator Data'!F25 * F$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="G28" s="42">
+      <c r="G28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G25), ISBLANK(G$4)), "", 'Indicator Data'!G25 * G$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="H28" s="42">
+      <c r="H28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H25), ISBLANK(H$4)), "", 'Indicator Data'!H25 * H$4)</f>
         <v>0.35</v>
       </c>
-      <c r="I28" s="42">
+      <c r="I28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I25), ISBLANK(I$4)), "", 'Indicator Data'!I25 * I$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="J28" s="42">
+      <c r="J28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J25), ISBLANK(J$4)), "", 'Indicator Data'!J25 * J$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="K28" s="42">
+      <c r="K28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K25), ISBLANK(K$4)), "", 'Indicator Data'!K25 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L28" s="42">
+      <c r="L28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L25), ISBLANK(L$4)), "", 'Indicator Data'!L25 * L$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="M28" s="42">
+      <c r="M28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M25), ISBLANK(M$4)), "", 'Indicator Data'!M25 * M$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="N28" s="42">
+      <c r="N28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N25), ISBLANK(N$4)), "", 'Indicator Data'!N25 * N$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="O28" s="42">
+      <c r="O28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O25), ISBLANK(O$4)), "", 'Indicator Data'!O25 * O$4)</f>
         <v>0.27</v>
       </c>
-      <c r="P28" s="42">
+      <c r="P28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P25), ISBLANK(P$4)), "", 'Indicator Data'!P25 * P$4)</f>
         <v>0.33750000000000002</v>
       </c>
-      <c r="Q28" s="42">
+      <c r="Q28" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q25), ISBLANK(Q$4)), "", 'Indicator Data'!Q25 * Q$4)</f>
         <v>0.33750000000000002</v>
       </c>
@@ -16405,63 +16428,63 @@
       <c r="B29" s="14" t="str">
         <v>Ternopilska</v>
       </c>
-      <c r="C29" s="42">
+      <c r="C29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C26), ISBLANK(C$4)), "", 'Indicator Data'!C26 * C$4)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="D29" s="42">
+      <c r="D29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D26), ISBLANK(D$4)), "", 'Indicator Data'!D26 * D$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E29" s="42">
+      <c r="E29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E26), ISBLANK(E$4)), "", 'Indicator Data'!E26 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F29" s="42">
+      <c r="F29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F26), ISBLANK(F$4)), "", 'Indicator Data'!F26 * F$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="G29" s="42">
+      <c r="G29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G26), ISBLANK(G$4)), "", 'Indicator Data'!G26 * G$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="H29" s="42">
+      <c r="H29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H26), ISBLANK(H$4)), "", 'Indicator Data'!H26 * H$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="I29" s="42">
+      <c r="I29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I26), ISBLANK(I$4)), "", 'Indicator Data'!I26 * I$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="J29" s="42">
+      <c r="J29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J26), ISBLANK(J$4)), "", 'Indicator Data'!J26 * J$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="K29" s="42">
+      <c r="K29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K26), ISBLANK(K$4)), "", 'Indicator Data'!K26 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L29" s="42">
+      <c r="L29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L26), ISBLANK(L$4)), "", 'Indicator Data'!L26 * L$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="M29" s="42">
+      <c r="M29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M26), ISBLANK(M$4)), "", 'Indicator Data'!M26 * M$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="N29" s="42">
+      <c r="N29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N26), ISBLANK(N$4)), "", 'Indicator Data'!N26 * N$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="O29" s="42">
+      <c r="O29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O26), ISBLANK(O$4)), "", 'Indicator Data'!O26 * O$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="P29" s="42">
+      <c r="P29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P26), ISBLANK(P$4)), "", 'Indicator Data'!P26 * P$4)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q29" s="42">
+      <c r="Q29" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q26), ISBLANK(Q$4)), "", 'Indicator Data'!Q26 * Q$4)</f>
         <v>0.1125</v>
       </c>
@@ -16473,63 +16496,63 @@
       <c r="B30" s="14" t="str">
         <v>Vinnytska</v>
       </c>
-      <c r="C30" s="42">
+      <c r="C30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C27), ISBLANK(C$4)), "", 'Indicator Data'!C27 * C$4)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="D30" s="42">
+      <c r="D30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D27), ISBLANK(D$4)), "", 'Indicator Data'!D27 * D$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="E30" s="42">
+      <c r="E30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E27), ISBLANK(E$4)), "", 'Indicator Data'!E27 * E$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="F30" s="42">
+      <c r="F30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F27), ISBLANK(F$4)), "", 'Indicator Data'!F27 * F$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="G30" s="42">
+      <c r="G30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G27), ISBLANK(G$4)), "", 'Indicator Data'!G27 * G$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H30" s="42">
+      <c r="H30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H27), ISBLANK(H$4)), "", 'Indicator Data'!H27 * H$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="I30" s="42">
+      <c r="I30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I27), ISBLANK(I$4)), "", 'Indicator Data'!I27 * I$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="J30" s="42">
+      <c r="J30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J27), ISBLANK(J$4)), "", 'Indicator Data'!J27 * J$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="K30" s="42">
+      <c r="K30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K27), ISBLANK(K$4)), "", 'Indicator Data'!K27 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L30" s="42">
+      <c r="L30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L27), ISBLANK(L$4)), "", 'Indicator Data'!L27 * L$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="M30" s="42">
+      <c r="M30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M27), ISBLANK(M$4)), "", 'Indicator Data'!M27 * M$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N30" s="42">
+      <c r="N30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N27), ISBLANK(N$4)), "", 'Indicator Data'!N27 * N$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="O30" s="42">
+      <c r="O30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O27), ISBLANK(O$4)), "", 'Indicator Data'!O27 * O$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="P30" s="42">
+      <c r="P30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P27), ISBLANK(P$4)), "", 'Indicator Data'!P27 * P$4)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q30" s="42">
+      <c r="Q30" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q27), ISBLANK(Q$4)), "", 'Indicator Data'!Q27 * Q$4)</f>
         <v>0.1125</v>
       </c>
@@ -16541,63 +16564,63 @@
       <c r="B31" s="14" t="str">
         <v>Volynska</v>
       </c>
-      <c r="C31" s="42">
+      <c r="C31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C28), ISBLANK(C$4)), "", 'Indicator Data'!C28 * C$4)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="D31" s="42">
+      <c r="D31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D28), ISBLANK(D$4)), "", 'Indicator Data'!D28 * D$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E31" s="42">
+      <c r="E31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E28), ISBLANK(E$4)), "", 'Indicator Data'!E28 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F31" s="42">
+      <c r="F31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F28), ISBLANK(F$4)), "", 'Indicator Data'!F28 * F$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="G31" s="42">
+      <c r="G31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G28), ISBLANK(G$4)), "", 'Indicator Data'!G28 * G$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="H31" s="42">
+      <c r="H31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H28), ISBLANK(H$4)), "", 'Indicator Data'!H28 * H$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="I31" s="42">
+      <c r="I31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I28), ISBLANK(I$4)), "", 'Indicator Data'!I28 * I$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="J31" s="42">
+      <c r="J31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J28), ISBLANK(J$4)), "", 'Indicator Data'!J28 * J$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="K31" s="42">
+      <c r="K31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K28), ISBLANK(K$4)), "", 'Indicator Data'!K28 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L31" s="42">
+      <c r="L31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L28), ISBLANK(L$4)), "", 'Indicator Data'!L28 * L$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="M31" s="42">
+      <c r="M31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M28), ISBLANK(M$4)), "", 'Indicator Data'!M28 * M$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="N31" s="42">
+      <c r="N31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N28), ISBLANK(N$4)), "", 'Indicator Data'!N28 * N$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="O31" s="42">
+      <c r="O31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O28), ISBLANK(O$4)), "", 'Indicator Data'!O28 * O$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="P31" s="42">
+      <c r="P31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P28), ISBLANK(P$4)), "", 'Indicator Data'!P28 * P$4)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q31" s="42">
+      <c r="Q31" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q28), ISBLANK(Q$4)), "", 'Indicator Data'!Q28 * Q$4)</f>
         <v>0.1125</v>
       </c>
@@ -16609,63 +16632,63 @@
       <c r="B32" s="14" t="str">
         <v>Zakarpatska</v>
       </c>
-      <c r="C32" s="42">
+      <c r="C32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C29), ISBLANK(C$4)), "", 'Indicator Data'!C29 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D32" s="42">
+      <c r="D32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D29), ISBLANK(D$4)), "", 'Indicator Data'!D29 * D$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="E32" s="42">
+      <c r="E32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E29), ISBLANK(E$4)), "", 'Indicator Data'!E29 * E$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="F32" s="42">
+      <c r="F32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F29), ISBLANK(F$4)), "", 'Indicator Data'!F29 * F$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="G32" s="42">
+      <c r="G32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G29), ISBLANK(G$4)), "", 'Indicator Data'!G29 * G$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H32" s="42">
+      <c r="H32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H29), ISBLANK(H$4)), "", 'Indicator Data'!H29 * H$4)</f>
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="I32" s="42">
+      <c r="I32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I29), ISBLANK(I$4)), "", 'Indicator Data'!I29 * I$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="J32" s="42">
+      <c r="J32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J29), ISBLANK(J$4)), "", 'Indicator Data'!J29 * J$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="K32" s="42">
+      <c r="K32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K29), ISBLANK(K$4)), "", 'Indicator Data'!K29 * K$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="L32" s="42">
+      <c r="L32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L29), ISBLANK(L$4)), "", 'Indicator Data'!L29 * L$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="M32" s="42">
+      <c r="M32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M29), ISBLANK(M$4)), "", 'Indicator Data'!M29 * M$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N32" s="42">
+      <c r="N32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N29), ISBLANK(N$4)), "", 'Indicator Data'!N29 * N$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="O32" s="42">
+      <c r="O32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O29), ISBLANK(O$4)), "", 'Indicator Data'!O29 * O$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="P32" s="42">
+      <c r="P32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P29), ISBLANK(P$4)), "", 'Indicator Data'!P29 * P$4)</f>
         <v>0.1125</v>
       </c>
-      <c r="Q32" s="42">
+      <c r="Q32" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q29), ISBLANK(Q$4)), "", 'Indicator Data'!Q29 * Q$4)</f>
         <v>0.1125</v>
       </c>
@@ -16677,63 +16700,63 @@
       <c r="B33" s="14" t="str">
         <v>Zaporizka</v>
       </c>
-      <c r="C33" s="42">
+      <c r="C33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C30), ISBLANK(C$4)), "", 'Indicator Data'!C30 * C$4)</f>
         <v>0.60000000000000009</v>
       </c>
-      <c r="D33" s="42">
+      <c r="D33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D30), ISBLANK(D$4)), "", 'Indicator Data'!D30 * D$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="E33" s="42">
+      <c r="E33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E30), ISBLANK(E$4)), "", 'Indicator Data'!E30 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F33" s="42">
+      <c r="F33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F30), ISBLANK(F$4)), "", 'Indicator Data'!F30 * F$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="G33" s="42">
+      <c r="G33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G30), ISBLANK(G$4)), "", 'Indicator Data'!G30 * G$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="H33" s="42" t="str">
+      <c r="H33" s="38" t="str">
         <f>IF(OR(ISBLANK('Indicator Data'!H30), ISBLANK(H$4)), "", 'Indicator Data'!H30 * H$4)</f>
         <v/>
       </c>
-      <c r="I33" s="42">
+      <c r="I33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I30), ISBLANK(I$4)), "", 'Indicator Data'!I30 * I$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="J33" s="42">
+      <c r="J33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J30), ISBLANK(J$4)), "", 'Indicator Data'!J30 * J$4)</f>
         <v>9.0000000000000011E-2</v>
       </c>
-      <c r="K33" s="42">
+      <c r="K33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K30), ISBLANK(K$4)), "", 'Indicator Data'!K30 * K$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="L33" s="42">
+      <c r="L33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L30), ISBLANK(L$4)), "", 'Indicator Data'!L30 * L$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="M33" s="42">
+      <c r="M33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M30), ISBLANK(M$4)), "", 'Indicator Data'!M30 * M$4)</f>
         <v>0.11250000000000002</v>
       </c>
-      <c r="N33" s="42">
+      <c r="N33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N30), ISBLANK(N$4)), "", 'Indicator Data'!N30 * N$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="O33" s="42">
+      <c r="O33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O30), ISBLANK(O$4)), "", 'Indicator Data'!O30 * O$4)</f>
         <v>0.36000000000000004</v>
       </c>
-      <c r="P33" s="42">
+      <c r="P33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P30), ISBLANK(P$4)), "", 'Indicator Data'!P30 * P$4)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q33" s="42">
+      <c r="Q33" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q30), ISBLANK(Q$4)), "", 'Indicator Data'!Q30 * Q$4)</f>
         <v>0.5625</v>
       </c>
@@ -16745,63 +16768,63 @@
       <c r="B34" s="14" t="str">
         <v>Zhytomyrska</v>
       </c>
-      <c r="C34" s="42">
+      <c r="C34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!C31), ISBLANK(C$4)), "", 'Indicator Data'!C31 * C$4)</f>
         <v>0.8</v>
       </c>
-      <c r="D34" s="42">
+      <c r="D34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!D31), ISBLANK(D$4)), "", 'Indicator Data'!D31 * D$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="E34" s="42">
+      <c r="E34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!E31), ISBLANK(E$4)), "", 'Indicator Data'!E31 * E$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="F34" s="42">
+      <c r="F34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!F31), ISBLANK(F$4)), "", 'Indicator Data'!F31 * F$4)</f>
         <v>0.27999999999999997</v>
       </c>
-      <c r="G34" s="42">
+      <c r="G34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!G31), ISBLANK(G$4)), "", 'Indicator Data'!G31 * G$4)</f>
         <v>0.13999999999999999</v>
       </c>
-      <c r="H34" s="42">
+      <c r="H34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!H31), ISBLANK(H$4)), "", 'Indicator Data'!H31 * H$4)</f>
         <v>0.20999999999999996</v>
       </c>
-      <c r="I34" s="42">
+      <c r="I34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!I31), ISBLANK(I$4)), "", 'Indicator Data'!I31 * I$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="J34" s="42">
+      <c r="J34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!J31), ISBLANK(J$4)), "", 'Indicator Data'!J31 * J$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="K34" s="42">
+      <c r="K34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!K31), ISBLANK(K$4)), "", 'Indicator Data'!K31 * K$4)</f>
         <v>4.5000000000000005E-2</v>
       </c>
-      <c r="L34" s="42">
+      <c r="L34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!L31), ISBLANK(L$4)), "", 'Indicator Data'!L31 * L$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="M34" s="42">
+      <c r="M34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!M31), ISBLANK(M$4)), "", 'Indicator Data'!M31 * M$4)</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="N34" s="42">
+      <c r="N34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!N31), ISBLANK(N$4)), "", 'Indicator Data'!N31 * N$4)</f>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="O34" s="42">
+      <c r="O34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!O31), ISBLANK(O$4)), "", 'Indicator Data'!O31 * O$4)</f>
         <v>0.27</v>
       </c>
-      <c r="P34" s="42">
+      <c r="P34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!P31), ISBLANK(P$4)), "", 'Indicator Data'!P31 * P$4)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="Q34" s="42">
+      <c r="Q34" s="38">
         <f>IF(OR(ISBLANK('Indicator Data'!Q31), ISBLANK(Q$4)), "", 'Indicator Data'!Q31 * Q$4)</f>
         <v>0.33750000000000002</v>
       </c>
@@ -16828,10 +16851,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8145C34-C5F9-9843-B221-F18C2AA209F7}">
+  <sheetPr>
+    <tabColor rgb="FFD9EAD3"/>
+  </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16839,7 +16865,7 @@
     <col min="1" max="1" width="12.1640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="14" customWidth="1"/>
     <col min="3" max="5" width="11" style="14" customWidth="1"/>
-    <col min="6" max="6" width="11" style="38" customWidth="1"/>
+    <col min="6" max="6" width="11" style="34" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
@@ -16896,7 +16922,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F2" s="37" t="str" cm="1">
+      <c r="F2" s="33" t="str" cm="1">
         <f t="array" ref="F2">IF(SUMPRODUCT(--(C2:E2&lt;&gt;""))=0, "-", SUM(C2:E2))</f>
         <v>-</v>
       </c>
@@ -16932,7 +16958,7 @@
 )</f>
         <v>0.72000000000000008</v>
       </c>
-      <c r="F3" s="37" cm="1">
+      <c r="F3" s="33" cm="1">
         <f t="array" ref="F3">IF(SUMPRODUCT(--(C3:E3&lt;&gt;""))=0, "-", SUM(C3:E3))</f>
         <v>2.5674999999999999</v>
       </c>
@@ -16968,7 +16994,7 @@
 )</f>
         <v>1.2375</v>
       </c>
-      <c r="F4" s="37" cm="1">
+      <c r="F4" s="33" cm="1">
         <f t="array" ref="F4">IF(SUMPRODUCT(--(C4:E4&lt;&gt;""))=0, "-", SUM(C4:E4))</f>
         <v>3.3549999999999995</v>
       </c>
@@ -17004,7 +17030,7 @@
 )</f>
         <v>0.5625</v>
       </c>
-      <c r="F5" s="37" cm="1">
+      <c r="F5" s="33" cm="1">
         <f t="array" ref="F5">IF(SUMPRODUCT(--(C5:E5&lt;&gt;""))=0, "-", SUM(C5:E5))</f>
         <v>2.085</v>
       </c>
@@ -17040,7 +17066,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F6" s="37" t="str" cm="1">
+      <c r="F6" s="33" t="str" cm="1">
         <f t="array" ref="F6">IF(SUMPRODUCT(--(C6:E6&lt;&gt;""))=0, "-", SUM(C6:E6))</f>
         <v>-</v>
       </c>
@@ -17076,7 +17102,7 @@
 )</f>
         <v>1.2375</v>
       </c>
-      <c r="F7" s="37" cm="1">
+      <c r="F7" s="33" cm="1">
         <f t="array" ref="F7">IF(SUMPRODUCT(--(C7:E7&lt;&gt;""))=0, "-", SUM(C7:E7))</f>
         <v>3.375</v>
       </c>
@@ -17112,7 +17138,7 @@
 )</f>
         <v>2.0475000000000003</v>
       </c>
-      <c r="F8" s="37" cm="1">
+      <c r="F8" s="33" cm="1">
         <f t="array" ref="F8">IF(SUMPRODUCT(--(C8:E8&lt;&gt;""))=0, "-", SUM(C8:E8))</f>
         <v>3.6850000000000005</v>
       </c>
@@ -17148,7 +17174,7 @@
 )</f>
         <v>0.76500000000000012</v>
       </c>
-      <c r="F9" s="37" cm="1">
+      <c r="F9" s="33" cm="1">
         <f t="array" ref="F9">IF(SUMPRODUCT(--(C9:E9&lt;&gt;""))=0, "-", SUM(C9:E9))</f>
         <v>2.52</v>
       </c>
@@ -17184,7 +17210,7 @@
 )</f>
         <v>1.8900000000000001</v>
       </c>
-      <c r="F10" s="37" cm="1">
+      <c r="F10" s="33" cm="1">
         <f t="array" ref="F10">IF(SUMPRODUCT(--(C10:E10&lt;&gt;""))=0, "-", SUM(C10:E10))</f>
         <v>4.2650000000000006</v>
       </c>
@@ -17220,7 +17246,7 @@
 )</f>
         <v>2.0700000000000003</v>
       </c>
-      <c r="F11" s="37" cm="1">
+      <c r="F11" s="33" cm="1">
         <f t="array" ref="F11">IF(SUMPRODUCT(--(C11:E11&lt;&gt;""))=0, "-", SUM(C11:E11))</f>
         <v>2.8625000000000003</v>
       </c>
@@ -17256,7 +17282,7 @@
 )</f>
         <v>0.5625</v>
       </c>
-      <c r="F12" s="37" cm="1">
+      <c r="F12" s="33" cm="1">
         <f t="array" ref="F12">IF(SUMPRODUCT(--(C12:E12&lt;&gt;""))=0, "-", SUM(C12:E12))</f>
         <v>2.27</v>
       </c>
@@ -17292,7 +17318,7 @@
 )</f>
         <v>0.81000000000000016</v>
       </c>
-      <c r="F13" s="37" cm="1">
+      <c r="F13" s="33" cm="1">
         <f t="array" ref="F13">IF(SUMPRODUCT(--(C13:E13&lt;&gt;""))=0, "-", SUM(C13:E13))</f>
         <v>2.1525000000000003</v>
       </c>
@@ -17328,7 +17354,7 @@
 )</f>
         <v>0.9900000000000001</v>
       </c>
-      <c r="F14" s="37" cm="1">
+      <c r="F14" s="33" cm="1">
         <f t="array" ref="F14">IF(SUMPRODUCT(--(C14:E14&lt;&gt;""))=0, "-", SUM(C14:E14))</f>
         <v>3.35</v>
       </c>
@@ -17340,33 +17366,33 @@
       <c r="B15" s="14" t="str">
         <v>Luhanska</v>
       </c>
-      <c r="C15" s="29" cm="1">
+      <c r="C15" s="29" t="str" cm="1">
         <f t="array" ref="C15">IF(
    SUMPRODUCT( ('Composite Indicator Matrix'!$1:$1 = C$1) * ('Composite Indicator Matrix'!20:20 &lt;&gt; "") ) = 0,
    "",
    SUMIF('Composite Indicator Matrix'!$1:$1, C$1, 'Composite Indicator Matrix'!20:20)
 )</f>
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="D15" s="29" cm="1">
+        <v/>
+      </c>
+      <c r="D15" s="29" t="str" cm="1">
         <f t="array" ref="D15">IF(
    SUMPRODUCT( ('Composite Indicator Matrix'!$1:$1 = D$1) * ('Composite Indicator Matrix'!20:20 &lt;&gt; "") ) = 0,
    "",
    SUMIF('Composite Indicator Matrix'!$1:$1, D$1, 'Composite Indicator Matrix'!20:20)
 )</f>
-        <v>0.42</v>
-      </c>
-      <c r="E15" s="29" cm="1">
+        <v/>
+      </c>
+      <c r="E15" s="29" t="str" cm="1">
         <f t="array" ref="E15">IF(
    SUMPRODUCT( ('Composite Indicator Matrix'!$1:$1 = E$1) * ('Composite Indicator Matrix'!20:20 &lt;&gt; "") ) = 0,
    "",
    SUMIF('Composite Indicator Matrix'!$1:$1, E$1, 'Composite Indicator Matrix'!20:20)
 )</f>
-        <v>0.90000000000000013</v>
-      </c>
-      <c r="F15" s="37" cm="1">
+        <v/>
+      </c>
+      <c r="F15" s="33" t="str" cm="1">
         <f t="array" ref="F15">IF(SUMPRODUCT(--(C15:E15&lt;&gt;""))=0, "-", SUM(C15:E15))</f>
-        <v>2.46</v>
+        <v>-</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -17400,7 +17426,7 @@
 )</f>
         <v>0.54</v>
       </c>
-      <c r="F16" s="37" cm="1">
+      <c r="F16" s="33" cm="1">
         <f t="array" ref="F16">IF(SUMPRODUCT(--(C16:E16&lt;&gt;""))=0, "-", SUM(C16:E16))</f>
         <v>2.5149999999999997</v>
       </c>
@@ -17436,7 +17462,7 @@
 )</f>
         <v>1.44</v>
       </c>
-      <c r="F17" s="37" cm="1">
+      <c r="F17" s="33" cm="1">
         <f t="array" ref="F17">IF(SUMPRODUCT(--(C17:E17&lt;&gt;""))=0, "-", SUM(C17:E17))</f>
         <v>3.7075</v>
       </c>
@@ -17472,7 +17498,7 @@
 )</f>
         <v/>
       </c>
-      <c r="F18" s="37" t="str" cm="1">
+      <c r="F18" s="33" t="str" cm="1">
         <f t="array" ref="F18">IF(SUMPRODUCT(--(C18:E18&lt;&gt;""))=0, "-", SUM(C18:E18))</f>
         <v>-</v>
       </c>
@@ -17508,7 +17534,7 @@
 )</f>
         <v>1.4849999999999999</v>
       </c>
-      <c r="F19" s="37" cm="1">
+      <c r="F19" s="33" cm="1">
         <f t="array" ref="F19">IF(SUMPRODUCT(--(C19:E19&lt;&gt;""))=0, "-", SUM(C19:E19))</f>
         <v>3.0375000000000001</v>
       </c>
@@ -17544,7 +17570,7 @@
 )</f>
         <v>1.3275000000000001</v>
       </c>
-      <c r="F20" s="37" cm="1">
+      <c r="F20" s="33" cm="1">
         <f t="array" ref="F20">IF(SUMPRODUCT(--(C20:E20&lt;&gt;""))=0, "-", SUM(C20:E20))</f>
         <v>3.1950000000000003</v>
       </c>
@@ -17580,7 +17606,7 @@
 )</f>
         <v>0.83250000000000013</v>
       </c>
-      <c r="F21" s="37" cm="1">
+      <c r="F21" s="33" cm="1">
         <f t="array" ref="F21">IF(SUMPRODUCT(--(C21:E21&lt;&gt;""))=0, "-", SUM(C21:E21))</f>
         <v>2.75</v>
       </c>
@@ -17616,7 +17642,7 @@
 )</f>
         <v>0.81</v>
       </c>
-      <c r="F22" s="37" cm="1">
+      <c r="F22" s="33" cm="1">
         <f t="array" ref="F22">IF(SUMPRODUCT(--(C22:E22&lt;&gt;""))=0, "-", SUM(C22:E22))</f>
         <v>2.355</v>
       </c>
@@ -17652,7 +17678,7 @@
 )</f>
         <v>1.2150000000000001</v>
       </c>
-      <c r="F23" s="37" cm="1">
+      <c r="F23" s="33" cm="1">
         <f t="array" ref="F23">IF(SUMPRODUCT(--(C23:E23&lt;&gt;""))=0, "-", SUM(C23:E23))</f>
         <v>3.2175000000000002</v>
       </c>
@@ -17688,7 +17714,7 @@
 )</f>
         <v>0.60750000000000004</v>
       </c>
-      <c r="F24" s="37" cm="1">
+      <c r="F24" s="33" cm="1">
         <f t="array" ref="F24">IF(SUMPRODUCT(--(C24:E24&lt;&gt;""))=0, "-", SUM(C24:E24))</f>
         <v>1.9300000000000002</v>
       </c>
@@ -17724,7 +17750,7 @@
 )</f>
         <v>0.63000000000000012</v>
       </c>
-      <c r="F25" s="37" cm="1">
+      <c r="F25" s="33" cm="1">
         <f t="array" ref="F25">IF(SUMPRODUCT(--(C25:E25&lt;&gt;""))=0, "-", SUM(C25:E25))</f>
         <v>2.4649999999999999</v>
       </c>
@@ -17760,7 +17786,7 @@
 )</f>
         <v>0.56250000000000011</v>
       </c>
-      <c r="F26" s="37" cm="1">
+      <c r="F26" s="33" cm="1">
         <f t="array" ref="F26">IF(SUMPRODUCT(--(C26:E26&lt;&gt;""))=0, "-", SUM(C26:E26))</f>
         <v>1.8375000000000004</v>
       </c>
@@ -17796,7 +17822,7 @@
 )</f>
         <v>0.54</v>
       </c>
-      <c r="F27" s="37" cm="1">
+      <c r="F27" s="33" cm="1">
         <f t="array" ref="F27">IF(SUMPRODUCT(--(C27:E27&lt;&gt;""))=0, "-", SUM(C27:E27))</f>
         <v>2.3174999999999999</v>
       </c>
@@ -17832,7 +17858,7 @@
 )</f>
         <v>1.62</v>
       </c>
-      <c r="F28" s="37" cm="1">
+      <c r="F28" s="33" cm="1">
         <f t="array" ref="F28">IF(SUMPRODUCT(--(C28:E28&lt;&gt;""))=0, "-", SUM(C28:E28))</f>
         <v>3.22</v>
       </c>
@@ -17868,7 +17894,7 @@
 )</f>
         <v>1.1025</v>
       </c>
-      <c r="F29" s="37" cm="1">
+      <c r="F29" s="33" cm="1">
         <f t="array" ref="F29">IF(SUMPRODUCT(--(C29:E29&lt;&gt;""))=0, "-", SUM(C29:E29))</f>
         <v>2.9275000000000002</v>
       </c>
@@ -17892,10 +17918,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1FCF2F-B32A-784C-A09B-6B7087BC2E46}">
+  <sheetPr>
+    <tabColor rgb="FFE6E6E6"/>
+  </sheetPr>
   <dimension ref="A1:D3131"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C2851" sqref="C2851"/>
+      <selection activeCell="D2861" sqref="D2861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Rename Total to Composite Risk Score and update UI
Replaces the 'Total' column with 'Composite Risk Score' throughout the codebase for clarity. Updates all relevant UI labels, table outputs, and sorting logic to reflect this change. Adds an Instructions tab to the UI and improves upload instructions for better user guidance.
</commit_message>
<xml_diff>
--- a/data/WHO Seasonal Risk Assessment Tool (SAMPLE).xlsx
+++ b/data/WHO Seasonal Risk Assessment Tool (SAMPLE).xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve.kerr/Documents/GitHub/riskassess/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05CB575A-F822-D647-B4B7-B3220AB565D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491591A8-36F8-3E49-9454-55ABDECEF931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17120" yWindow="-20980" windowWidth="38400" windowHeight="20980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="18960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="README" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Indicator Metadata" sheetId="8" r:id="rId2"/>
     <sheet name="Indicator Data" sheetId="12" r:id="rId3"/>
     <sheet name="Pillar Weights" sheetId="15" r:id="rId4"/>
@@ -10436,7 +10436,8 @@
     <t>Administrative Level 1</t>
   </si>
   <si>
-    <t>TOTAL</t>
+    <t>Composite 
+Risk Scores</t>
   </si>
 </sst>
 </file>
@@ -10664,6 +10665,7 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -10676,7 +10678,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11688,7 +11689,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11704,11 +11705,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="238.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
     </row>
     <row r="3" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -11766,11 +11767,11 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11790,7 +11791,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12375,7 +12376,7 @@
         <v>LOCC</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="137" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="138" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>49</v>
       </c>
@@ -14475,7 +14476,7 @@
   </sheetPr>
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="118" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="118" workbookViewId="0">
       <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
@@ -15603,7 +15604,7 @@
         <f>IF(OR(ISBLANK('Indicator Data'!Q13), ISBLANK(Q$4)), "", 'Indicator Data'!Q13 * Q$4)</f>
         <v>0.5625</v>
       </c>
-      <c r="T16" s="44"/>
+      <c r="T16" s="40"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="str">
@@ -16857,7 +16858,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16865,27 +16866,27 @@
     <col min="1" max="1" width="12.1640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="14" customWidth="1"/>
     <col min="3" max="5" width="11" style="14" customWidth="1"/>
-    <col min="6" max="6" width="11" style="34" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="34" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" s="13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>3386</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="18" t="s">
         <v>3385</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="18" t="s">
         <v>3389</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="22" t="s">
         <v>3395</v>
       </c>
     </row>

</xml_diff>